<commit_message>
Complete wikidata links in 1701 places
</commit_message>
<xml_diff>
--- a/inferences/places-1644.xlsx
+++ b/inferences/places-1644.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -560,7 +560,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>no wikidata.Jen-houo, hoje: Renhe, 仁和县, Historical county name. coordinate: 30.448897N, 120.307504E</t>
+          <t>Jen-houo, hoje: Renhe, 仁和县, Historical county name. coordinate: 30.448897N, 120.307504E</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>in the Chinese translation it is recognized as “遂州”, which is wrong, both phonetically and geographically. In Dehergne(1957), it is noted as "衢州".K'iu-tcheou, hoje:Quzhou, 衢州, , in the Chinese translation it is recognized as “遂州”, which is wrong, both phonetically and geographically. In Dehergne(1957), it is noted as "衢州".</t>
+          <t>K'iu-tcheou, hoje:Quzhou, 衢州, , in the Chinese translation it is recognized as “遂州”, which is wrong, both phonetically and geographically. In Dehergne(1957), it is noted as "衢州".</t>
         </is>
       </c>
     </row>
@@ -695,8 +695,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>"""
-               The place name in the book Dehergne(1973) is "Kaoshan", and in the Chinese translation it is recognized as “高山”. But this place cannot be found. According to Dehergne(1957), it probably shoud be "Kashan 嘉善", which means in the 1973 book, this place is wrongly spelled by mistake."""Kia-chan, hoje: Jiashan, 嘉善, Kaosham</t>
+          <t>Kia-chan, hoje: Jiashan, 嘉善, Kaosham</t>
         </is>
       </c>
     </row>
@@ -1119,14 +1118,10 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Q11146687</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>bourg de Hungtang, hoje: Hongtang, 洪塘, , in the Chinese translation it is written as “宏塘”, and in Dehergne(1957) it is "洪堂". But actually this place is written with the characters "洪塘".</t>
-        </is>
-      </c>
+          <t>No wikidata</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1340,7 +1335,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>et la baie d'Amoy entre Changchow et Chüanchow v. 1616Zhangzhou, hoje:Zhangzhou, 漳州, Changchow (Lungki)</t>
+          <t>Zhangzhou, hoje:Zhangzhou, 漳州, Changchow (Lungki)</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1362,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>"""in the Chinese translation it is recognized as “章浦”（漳浦）, which is wrong. It should be "后坂", because "Aupua" corresponds to the pronunciation of "后坂" in the southern Fujian dialect, and in Dehergne(1957), it has another transcription "Heupuen", which prooves it coordinate：24.50213852506329N, 117.6917197408656E"""hoje: Houban, 后坂, (@geonames:1977135)Au-poa,Heupuen</t>
+          <t>hoje: Houban, 后坂, (@geonames:1977135)Au-poa,Heupuen</t>
         </is>
       </c>
     </row>
@@ -2173,7 +2168,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">bourg de Cabaran hoje:Yilan, 葛子兰(宜兰), @wikidata:Q680842 Now it is called 宜兰Ki-long, Jilong, hoje:Keelung, 基隆, </t>
+          <t xml:space="preserve">Ki-long, Jilong, hoje:Keelung, 基隆, </t>
         </is>
       </c>
     </row>
@@ -2223,7 +2218,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>"""In the Chinese translation it is recognized as “塔巴里”, in Dehergne(1957) it is noted as "大包里", which cannot be found in the map. As Dehergne(1957) said it is at "Peninsule de Masu, à 1 lieue nord-ouest de San Salvador (社寮)", coordinate of Peninsule Masu: 25.201218764354735N, 121.68618375811317E"""hoje：大包里</t>
+          <t>hoje：大包里</t>
         </is>
       </c>
     </row>
@@ -2300,7 +2295,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">(12 ou 13 chrétientés en 1641)hoje:Henan, 河南, </t>
+          <t xml:space="preserve">hoje:Henan, 河南, </t>
         </is>
       </c>
     </row>
@@ -2381,7 +2376,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Today it is named 商丘 Shanqiu. Wikidata code is that of ShangqiuKoei-té,Kueite, hoje: Guide, 归德, </t>
+          <t xml:space="preserve">Koei-té,Kueite, hoje: Guide, 归德, </t>
         </is>
       </c>
     </row>
@@ -2404,7 +2399,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Former province of China, corresponding to modern-day Hubei and Hunan provincesHuguang?, Hou-Quang, hoje:Huguang,湖广, </t>
+          <t xml:space="preserve">Huguang?, Hou-Quang, hoje:Huguang,湖广, </t>
         </is>
       </c>
     </row>
@@ -2593,7 +2588,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">In the Chinese translation it is recogniazed as “蕲水”, which is also a place at that area, but according to the phonetic, it should be "蕲州", which is also noted in Dehergne(1957).do Hupei?, K'i-tcheou,Chichou, hoje: Qizhou, 蕲州, </t>
+          <t xml:space="preserve">do Hupei?, K'i-tcheou,Chichou, hoje: Qizhou, 蕲州, </t>
         </is>
       </c>
     </row>
@@ -2922,11 +2917,7 @@
           <t>No wikidata</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>In Dehergne(1957, p51): "Chrétienté au Wuyüan (Ou-yuen) hien, à la frontière du Kiangsi, et se nomme Tungmen, à l'ouest du Wuyüan, route de Kingtehchen." in the Chinese translation it is recogniazed as “东门村”, but it seems that there is no 东门村 in this area.</t>
-        </is>
-      </c>
+      <c r="E94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3406,7 +3397,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">松江府 is an ancient superior prefecture of chinaSong-kiang,Sungching, hoje: Songjiang, 松江, </t>
+          <t xml:space="preserve">Song-kiang,Sungching, hoje: Songjiang, 松江, </t>
         </is>
       </c>
     </row>
@@ -3595,7 +3586,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">nombreux bourgsChang-hai, hoje: Shanghai, 上海, </t>
+          <t xml:space="preserve">Chang-hai, hoje: Shanghai, 上海, </t>
         </is>
       </c>
     </row>
@@ -3649,7 +3640,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">In the Chinses translation it is written as “七堡”, which should be “七宝”Tsi-pao,Chipao, hoje: Qibao, 七宝, </t>
+          <t xml:space="preserve">Tsi-pao,Chipao, hoje: Qibao, 七宝, </t>
         </is>
       </c>
     </row>
@@ -4096,7 +4087,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>, In the Chinese translation, Lappa is recognized as “浪白”, acutuallythe Portugese people called “湾仔 Wanzai” as Lappa. 湾仔 is now a place in Zhuhai.Lapa,Wantchai, hoje: Wanzai, 湾仔, Lappa (Wantchai)</t>
+          <t>Lapa,Wantchai, hoje: Wanzai, 湾仔, Lappa (Wantchai)</t>
         </is>
       </c>
     </row>
@@ -4231,7 +4222,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Qiongzhou is the ancient name of Hainan Island. Wikidata code same as Hainan Island.K'iong-tcheou,Chiungchou, hoje: Qiongzhou, 琼州, Kiungchow (île de Hainan)</t>
+          <t>K'iong-tcheou,Chiungchou, hoje: Qiongzhou, 琼州, Kiungchow (île de Hainan)</t>
         </is>
       </c>
     </row>
@@ -4447,7 +4438,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>où première église bâtie hors de Macao, en 1603Cinçun, hoje: Jingcun, 靖村, coordinate:24.840448198893206N, 113.54394322209676E. In the original book (Dehergne, 1973), it is written as "Tsintsun" (without g), which is wrongly spelled. In Dehergne(1973), it is written as Tsingtsun, with the Chinese name 靖村 noted. It is "à une heure et demie de marche au nord-ouest de Siuchow." In the Chinese traslation, it is recognized as "青村", which is wrong.</t>
+          <t>Cinçun, hoje: Jingcun, 靖村, coordinate:24.840448198893206N, 113.54394322209676E. In the original book (Dehergne, 1973), it is written as "Tsintsun" (without g), which is wrongly spelled. In Dehergne(1973), it is written as Tsingtsun, with the Chinese name 靖村 noted. It is "à une heure et demie de marche au nord-ouest de Siuchow." In the Chinese traslation, it is recognized as "青村", which is wrong.</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4465,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>tous bourgs évangélisés avant 1603Vançun, hoje: Huangcun, 黄村, coordinate: 24.900778941203768N, 113.60398607001083E Dehergne(1957): "à une heure de chemin au nord de Shiuchow".</t>
+          <t>Vançun, hoje: Huangcun, 黄村, coordinate: 24.900778941203768N, 113.60398607001083E Dehergne(1957): "à une heure de chemin au nord de Shiuchow".</t>
         </is>
       </c>
     </row>
@@ -4501,7 +4492,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>tous bourgs évangélisés avant 1603Hwanghsiaping, hoje: Vankaxen, 黄下坪？, In the Chinese translation, it is recognized as "黄下坪". Dehergne(1957):"Hwanghsiaping (" Vankaxen ") à 15 li à l'ouest de Shiuchow." But it cannot be found in the map.</t>
+          <t>Hwanghsiaping, hoje: Vankaxen, 黄下坪？, In the Chinese translation, it is recognized as "黄下坪". Dehergne(1957):"Hwanghsiaping (" Vankaxen ") à 15 li à l'ouest de Shiuchow." But it cannot be found in the map.</t>
         </is>
       </c>
     </row>
@@ -4528,7 +4519,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>tous bourgs évangélisés avant 1603Mochi, hoje: Madigang, 麻地岗, In the Chinese translation, it is recognized as “末岗”, but in Dehergne(1957), it is noted as “麻地岗”. coordinate: 24.68899887552694N, 113.57599418283718E</t>
+          <t>Mochi, hoje: Madigang, 麻地岗, In the Chinese translation, it is recognized as “末岗”, but in Dehergne(1957), it is noted as “麻地岗”. coordinate: 24.68899887552694N, 113.57599418283718E</t>
         </is>
       </c>
     </row>
@@ -4555,7 +4546,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>tous bourgs évangélisés avant 1603Yang-hiang, hoje: 杨姓村</t>
+          <t>Yang-hiang, hoje: 杨姓村</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4596,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t xml:space="preserve">nadaKoei-Tcheou, hoje: Guizhou, 贵州, </t>
+          <t xml:space="preserve">Koei-Tcheou, hoje: Guizhou, 贵州, </t>
         </is>
       </c>
     </row>
@@ -4651,7 +4642,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>En 1637 16 chrétientés et 14 oratoires autour de Pékinhoje: 北京, Peking (Shuntien) (1598), 1601</t>
+          <t>hoje: 北京, Peking (Shuntien) (1598), 1601</t>
         </is>
       </c>
     </row>
@@ -4786,12 +4777,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t xml:space="preserve">"""Chengting fou is Zhengding Fu （正定府） in Hebei province
-                     with the wikidata code Q11123399. However, as a historical
-                     administrative division, its wikidata code does not include
-                     its geographical information,  we  use the wikidata code
-                     of Zhengdign County (正定县) Q197678, because this is where
-                     it is in the present day."""Tcheng-ting, hoje: Zhengding, 正定, </t>
+          <t xml:space="preserve">Tcheng-ting, hoje: Zhengding, 正定, </t>
         </is>
       </c>
     </row>
@@ -5429,11 +5415,7 @@
           <t>No wikidata</t>
         </is>
       </c>
-      <c r="E188" t="inlineStr">
-        <is>
-          <t>In Dehergne(1957), there is no "Kwanchang". In the Chinese translation, it is recognized as “官昌”，but cannot be found in the map.</t>
-        </is>
-      </c>
+      <c r="E188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -5670,7 +5652,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>?Dehergne(1957)did not give the Chinese name of Peichingtien.In the Chinese translation, it is recognized as “北辛店村”，but the pronunciation dose not match. In addition, the “北辛店村”of Shandong is far from Dongchang.</t>
+          <t>Dehergne(1957)did not give the Chinese name of Peichingtien.In the Chinese translation, it is recognized as “北辛店村”，but the pronunciation dose not match. In addition, the “北辛店村”of Shandong is far from Dongchang.</t>
         </is>
       </c>
     </row>
@@ -5828,7 +5810,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Kiao-tou and Tungyüanfang are the same place. The Chinese translation recognized it as “贾都”, which might be wrong, as “贾都” cannot be found.Kiao-tou (ou Tungyiianfang)</t>
+          <t>Kiao-tou (ou Tungyiianfang)</t>
         </is>
       </c>
     </row>
@@ -5988,11 +5970,7 @@
           <t>No wikidata</t>
         </is>
       </c>
-      <c r="E209" t="inlineStr">
-        <is>
-          <t>In Dehergne(1957), it is noted as "小塞子", and in the Chinese translation, it is recognized as "小寨子村"。 But both places are not “ près de Cheng” as said in Dehergne(1957).</t>
-        </is>
-      </c>
+      <c r="E209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -6094,7 +6072,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mienchow is an historical administrative division, now it is located in the city of Mianyang.The Wikidata code also refers to that of Mianyang: Q426130Mien tcheou, hoje: Mianzhou, 绵州, hoje:  </t>
+          <t xml:space="preserve">Mien tcheou, hoje: Mianzhou, 绵州, hoje:  </t>
         </is>
       </c>
     </row>

</xml_diff>